<commit_message>
error: mCSB_11 & 12 conflict
</commit_message>
<xml_diff>
--- a/selenium/output.xlsx
+++ b/selenium/output.xlsx
@@ -1,118 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snp/web/Selenium/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE41BA-992D-5B48-9130-CF79F79DD0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
-  <si>
-    <t>일련번호</t>
-  </si>
-  <si>
-    <t>학교명</t>
-  </si>
-  <si>
-    <t>관할교육청</t>
-  </si>
-  <si>
-    <t>검색명*</t>
-  </si>
-  <si>
-    <t>졸업자</t>
-  </si>
-  <si>
-    <t>일반고</t>
-  </si>
-  <si>
-    <t>특성화고</t>
-  </si>
-  <si>
-    <t>과학고</t>
-  </si>
-  <si>
-    <t>외고/국제고</t>
-  </si>
-  <si>
-    <t>예고/체고</t>
-  </si>
-  <si>
-    <t>마이스터고</t>
-  </si>
-  <si>
-    <t>자사고</t>
-  </si>
-  <si>
-    <t>자공고</t>
-  </si>
-  <si>
-    <t>기타</t>
-  </si>
-  <si>
-    <t>취업자</t>
-  </si>
-  <si>
-    <t>무직자 및 미상</t>
-  </si>
-  <si>
-    <t>교육기관 진학 
-(학력 미인정)</t>
-  </si>
-  <si>
-    <t>교육기관 진학
-(학력 미인정)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,31 +78,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -468,136 +464,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col width="9.5" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="8.5" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="11.5" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="11.5" customWidth="1" style="6" min="5" max="5"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="6" max="7"/>
+    <col width="9.5" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="9" max="9"/>
+    <col width="12.33203125" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
+    <col width="10.33203125" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="11.5" bestFit="1" customWidth="1" style="1" min="12" max="12"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="13" max="14"/>
+    <col width="5.5" bestFit="1" customWidth="1" style="1" min="15" max="15"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="16" max="16"/>
+    <col width="14" bestFit="1" customWidth="1" style="1" min="17" max="17"/>
+    <col width="14.33203125" bestFit="1" customWidth="1" style="1" min="18" max="18"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="19" max="20"/>
+    <col width="9.5" bestFit="1" customWidth="1" style="1" min="21" max="21"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="22" max="22"/>
+    <col width="12.33203125" bestFit="1" customWidth="1" style="1" min="23" max="23"/>
+    <col width="10.33203125" bestFit="1" customWidth="1" style="1" min="24" max="24"/>
+    <col width="11.5" bestFit="1" customWidth="1" style="1" min="25" max="25"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="26" max="27"/>
+    <col width="5.5" bestFit="1" customWidth="1" style="1" min="28" max="28"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="1" min="29" max="29"/>
+    <col width="14" bestFit="1" customWidth="1" style="1" min="30" max="30"/>
+    <col width="14.33203125" bestFit="1" customWidth="1" style="1" min="31" max="31"/>
+    <col width="10.83203125" customWidth="1" style="1" min="32" max="33"/>
+    <col width="10.83203125" customWidth="1" style="1" min="34" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+    <row r="1" ht="34" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>일련번호</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>검색명*</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>학교명</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>관할교육청</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>대표번호*</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>졸업자</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>일반고</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>특성화고</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>과학고</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>외고/국제고</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>예고/체고</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>마이스터고</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>자사고</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>자공고</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>취업자</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>교육기관 진학 
+(학력 미인정)</t>
+        </is>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
+          <t>무직자 및 미상</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>졸업자</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>일반고</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>특성화고</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>과학고</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>외고/국제고</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>예고/체고</t>
+        </is>
+      </c>
+      <c r="Y1" s="3" t="inlineStr">
+        <is>
+          <t>마이스터고</t>
+        </is>
+      </c>
+      <c r="Z1" s="3" t="inlineStr">
+        <is>
+          <t>자사고</t>
+        </is>
+      </c>
+      <c r="AA1" s="3" t="inlineStr">
+        <is>
+          <t>자공고</t>
+        </is>
+      </c>
+      <c r="AB1" s="3" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="AC1" s="3" t="inlineStr">
+        <is>
+          <t>취업자</t>
+        </is>
+      </c>
+      <c r="AD1" s="5" t="inlineStr">
+        <is>
+          <t>교육기관 진학
+(학력 미인정)</t>
+        </is>
+      </c>
+      <c r="AE1" s="3" t="inlineStr">
+        <is>
+          <t>무직자 및 미상</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>15</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>서울 가락중학교</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
       </c>
     </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>